<commit_message>
changes made in IO process
</commit_message>
<xml_diff>
--- a/momentum_strategy_results.xlsx
+++ b/momentum_strategy_results.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,7 +504,7 @@
         <v>13.55</v>
       </c>
       <c r="C2" t="n">
-        <v>6.04</v>
+        <v>6.039999961853027</v>
       </c>
       <c r="D2" t="n">
         <v>7.5</v>
@@ -541,7 +541,7 @@
         <v>11.66</v>
       </c>
       <c r="C3" t="n">
-        <v>6.04</v>
+        <v>6.039999961853027</v>
       </c>
       <c r="D3" t="n">
         <v>5.62</v>
@@ -578,7 +578,7 @@
         <v>11.52</v>
       </c>
       <c r="C4" t="n">
-        <v>6.04</v>
+        <v>6.039999961853027</v>
       </c>
       <c r="D4" t="n">
         <v>5.48</v>
@@ -615,7 +615,7 @@
         <v>8.470000000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>6.04</v>
+        <v>6.039999961853027</v>
       </c>
       <c r="D5" t="n">
         <v>2.43</v>
@@ -652,7 +652,7 @@
         <v>6.99</v>
       </c>
       <c r="C6" t="n">
-        <v>6.04</v>
+        <v>6.039999961853027</v>
       </c>
       <c r="D6" t="n">
         <v>0.9399999999999999</v>
@@ -677,191 +677,6 @@
       </c>
       <c r="K6" t="n">
         <v>0.45</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>10-10-10-pct0.1-ceiling500000</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>6.32</v>
-      </c>
-      <c r="C7" t="n">
-        <v>6.04</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.27</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>41668</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>45656</v>
-      </c>
-      <c r="G7" t="n">
-        <v>270</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.0098</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.0015</v>
-      </c>
-      <c r="J7" t="n">
-        <v>76865</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>10-10-10-pct0.2-ceiling1200</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>7.47</v>
-      </c>
-      <c r="C8" t="n">
-        <v>6.04</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1.43</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>41668</v>
-      </c>
-      <c r="F8" s="2" t="n">
-        <v>45656</v>
-      </c>
-      <c r="G8" t="n">
-        <v>270</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.0098</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.0015</v>
-      </c>
-      <c r="J8" t="n">
-        <v>47104</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>10-10-10-pct0.2-ceiling1800</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>6.75</v>
-      </c>
-      <c r="C9" t="n">
-        <v>6.04</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>41668</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>45656</v>
-      </c>
-      <c r="G9" t="n">
-        <v>270</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.0094</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.0015</v>
-      </c>
-      <c r="J9" t="n">
-        <v>67897</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>10-10-10-pct0.2-ceiling500000</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>5.93</v>
-      </c>
-      <c r="C10" t="n">
-        <v>6.04</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-0.12</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>41668</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>45656</v>
-      </c>
-      <c r="G10" t="n">
-        <v>270</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.008999999999999999</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.0012</v>
-      </c>
-      <c r="J10" t="n">
-        <v>385426</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>10-10-10-pct0.3-ceiling1200</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>6.02</v>
-      </c>
-      <c r="C11" t="n">
-        <v>6.04</v>
-      </c>
-      <c r="D11" t="n">
-        <v>-0.03</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>41668</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>45656</v>
-      </c>
-      <c r="G11" t="n">
-        <v>270</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.0089</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="J11" t="n">
-        <v>77090</v>
-      </c>
-      <c r="K11" t="n">
-        <v>0.38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>